<commit_message>
core data generation logic done
</commit_message>
<xml_diff>
--- a/41467_2016_BFncomms12544_MOESM1319_ESM.xlsx
+++ b/41467_2016_BFncomms12544_MOESM1319_ESM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvesboutellier/Coding/Ceven/map-tinkering/eDNA-data-generation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28505CA-135B-3142-87B7-8CD6804992A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12870"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplemental Data 3" sheetId="3" r:id="rId1"/>
@@ -2196,7 +2202,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -2528,19 +2534,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:K257" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A2:K257" totalsRowShown="0" headerRowDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" name="Phylum" dataDxfId="10"/>
-    <tableColumn id="2" name="Class" dataDxfId="9"/>
-    <tableColumn id="3" name="Order" dataDxfId="8"/>
-    <tableColumn id="4" name="Family" dataDxfId="7"/>
-    <tableColumn id="5" name="Genus" dataDxfId="6"/>
-    <tableColumn id="6" name="Species" dataDxfId="5"/>
-    <tableColumn id="7" name="Habitat" dataDxfId="4"/>
-    <tableColumn id="8" name="Number of Sequences" dataDxfId="3"/>
-    <tableColumn id="9" name="Average of % of identical matches" dataDxfId="2"/>
-    <tableColumn id="10" name="Average reference alignment length" dataDxfId="1"/>
-    <tableColumn id="11" name="Geographic confirmation source" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Phylum" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Class" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Order" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Family" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Genus" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Species" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Habitat" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Number of Sequences" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Average of % of identical matches" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Average reference alignment length" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Geographic confirmation source" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2801,36 +2807,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" customWidth="1"/>
-    <col min="11" max="11" width="118.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" customWidth="1"/>
+    <col min="11" max="11" width="118.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="61.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>716</v>
       </c>
@@ -2845,7 +2851,7 @@
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>203</v>
       </c>
@@ -2880,7 +2886,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2915,7 +2921,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -2950,7 +2956,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -2985,7 +2991,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
@@ -3020,7 +3026,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
@@ -3055,7 +3061,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
@@ -3090,7 +3096,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
@@ -3125,7 +3131,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
@@ -3160,7 +3166,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
@@ -3195,7 +3201,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -3230,7 +3236,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>1</v>
       </c>
@@ -3265,7 +3271,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
@@ -3300,7 +3306,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>1</v>
       </c>
@@ -3335,7 +3341,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>1</v>
       </c>
@@ -3370,7 +3376,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>1</v>
       </c>
@@ -3405,7 +3411,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>1</v>
       </c>
@@ -3440,7 +3446,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>1</v>
       </c>
@@ -3475,7 +3481,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>1</v>
       </c>
@@ -3510,7 +3516,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>4</v>
       </c>
@@ -3545,7 +3551,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>4</v>
       </c>
@@ -3580,7 +3586,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>4</v>
       </c>
@@ -3615,7 +3621,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>4</v>
       </c>
@@ -3650,7 +3656,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>4</v>
       </c>
@@ -3685,7 +3691,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>4</v>
       </c>
@@ -3720,7 +3726,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>4</v>
       </c>
@@ -3755,7 +3761,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>4</v>
       </c>
@@ -3790,7 +3796,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>4</v>
       </c>
@@ -3825,7 +3831,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>4</v>
       </c>
@@ -3860,7 +3866,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>4</v>
       </c>
@@ -3895,7 +3901,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>4</v>
       </c>
@@ -3930,7 +3936,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>4</v>
       </c>
@@ -3965,7 +3971,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>4</v>
       </c>
@@ -4000,7 +4006,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>4</v>
       </c>
@@ -4035,7 +4041,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>4</v>
       </c>
@@ -4070,7 +4076,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>4</v>
       </c>
@@ -4105,7 +4111,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>4</v>
       </c>
@@ -4140,7 +4146,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>4</v>
       </c>
@@ -4175,7 +4181,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>4</v>
       </c>
@@ -4210,7 +4216,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>4</v>
       </c>
@@ -4245,7 +4251,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>4</v>
       </c>
@@ -4280,7 +4286,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>4</v>
       </c>
@@ -4315,7 +4321,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>4</v>
       </c>
@@ -4350,7 +4356,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>4</v>
       </c>
@@ -4385,7 +4391,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>4</v>
       </c>
@@ -4420,7 +4426,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>4</v>
       </c>
@@ -4455,7 +4461,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>4</v>
       </c>
@@ -4490,7 +4496,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>4</v>
       </c>
@@ -4525,7 +4531,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>4</v>
       </c>
@@ -4560,7 +4566,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>4</v>
       </c>
@@ -4595,7 +4601,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>4</v>
       </c>
@@ -4630,7 +4636,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>4</v>
       </c>
@@ -4665,7 +4671,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>4</v>
       </c>
@@ -4700,7 +4706,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>4</v>
       </c>
@@ -4735,7 +4741,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>4</v>
       </c>
@@ -4770,7 +4776,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>4</v>
       </c>
@@ -4805,7 +4811,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>4</v>
       </c>
@@ -4840,7 +4846,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>4</v>
       </c>
@@ -4875,7 +4881,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>4</v>
       </c>
@@ -4910,7 +4916,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>4</v>
       </c>
@@ -4945,7 +4951,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>4</v>
       </c>
@@ -4980,7 +4986,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>4</v>
       </c>
@@ -5015,7 +5021,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>4</v>
       </c>
@@ -5050,7 +5056,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>4</v>
       </c>
@@ -5085,7 +5091,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>4</v>
       </c>
@@ -5120,7 +5126,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>4</v>
       </c>
@@ -5155,7 +5161,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>4</v>
       </c>
@@ -5190,7 +5196,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>4</v>
       </c>
@@ -5225,7 +5231,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
         <v>4</v>
       </c>
@@ -5260,7 +5266,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>4</v>
       </c>
@@ -5295,7 +5301,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>4</v>
       </c>
@@ -5330,7 +5336,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
         <v>4</v>
       </c>
@@ -5365,7 +5371,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
         <v>4</v>
       </c>
@@ -5400,7 +5406,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
         <v>4</v>
       </c>
@@ -5435,7 +5441,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
         <v>4</v>
       </c>
@@ -5470,7 +5476,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>4</v>
       </c>
@@ -5505,7 +5511,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
         <v>4</v>
       </c>
@@ -5540,7 +5546,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>4</v>
       </c>
@@ -5575,7 +5581,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
         <v>4</v>
       </c>
@@ -5610,7 +5616,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
         <v>4</v>
       </c>
@@ -5645,7 +5651,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
         <v>4</v>
       </c>
@@ -5680,7 +5686,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
         <v>4</v>
       </c>
@@ -5715,7 +5721,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>4</v>
       </c>
@@ -5750,7 +5756,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
         <v>4</v>
       </c>
@@ -5785,7 +5791,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>4</v>
       </c>
@@ -5820,7 +5826,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>4</v>
       </c>
@@ -5855,7 +5861,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>4</v>
       </c>
@@ -5890,7 +5896,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>4</v>
       </c>
@@ -5925,7 +5931,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
         <v>4</v>
       </c>
@@ -5960,7 +5966,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>4</v>
       </c>
@@ -5995,7 +6001,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>4</v>
       </c>
@@ -6030,7 +6036,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>4</v>
       </c>
@@ -6065,7 +6071,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>4</v>
       </c>
@@ -6100,7 +6106,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>4</v>
       </c>
@@ -6135,7 +6141,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>4</v>
       </c>
@@ -6170,7 +6176,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
         <v>4</v>
       </c>
@@ -6205,7 +6211,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
         <v>4</v>
       </c>
@@ -6240,7 +6246,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
         <v>4</v>
       </c>
@@ -6275,7 +6281,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
         <v>4</v>
       </c>
@@ -6310,7 +6316,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
         <v>4</v>
       </c>
@@ -6345,7 +6351,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
         <v>4</v>
       </c>
@@ -6380,7 +6386,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
         <v>4</v>
       </c>
@@ -6415,7 +6421,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
         <v>4</v>
       </c>
@@ -6450,7 +6456,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
         <v>4</v>
       </c>
@@ -6485,7 +6491,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
         <v>4</v>
       </c>
@@ -6520,7 +6526,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
         <v>4</v>
       </c>
@@ -6555,7 +6561,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
         <v>4</v>
       </c>
@@ -6590,7 +6596,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
         <v>4</v>
       </c>
@@ -6625,7 +6631,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
         <v>4</v>
       </c>
@@ -6660,7 +6666,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
         <v>4</v>
       </c>
@@ -6695,7 +6701,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
         <v>4</v>
       </c>
@@ -6730,7 +6736,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
         <v>4</v>
       </c>
@@ -6765,7 +6771,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
         <v>4</v>
       </c>
@@ -6800,7 +6806,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
         <v>4</v>
       </c>
@@ -6835,7 +6841,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
         <v>4</v>
       </c>
@@ -6870,7 +6876,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
         <v>4</v>
       </c>
@@ -6905,7 +6911,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
         <v>4</v>
       </c>
@@ -6940,7 +6946,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
         <v>4</v>
       </c>
@@ -6975,7 +6981,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
         <v>4</v>
       </c>
@@ -7010,7 +7016,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
         <v>4</v>
       </c>
@@ -7045,7 +7051,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
         <v>4</v>
       </c>
@@ -7080,7 +7086,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
         <v>4</v>
       </c>
@@ -7115,7 +7121,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
         <v>4</v>
       </c>
@@ -7150,7 +7156,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
         <v>4</v>
       </c>
@@ -7185,7 +7191,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
         <v>4</v>
       </c>
@@ -7220,7 +7226,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
         <v>4</v>
       </c>
@@ -7255,7 +7261,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
         <v>4</v>
       </c>
@@ -7290,7 +7296,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="s">
         <v>4</v>
       </c>
@@ -7325,7 +7331,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
         <v>4</v>
       </c>
@@ -7360,7 +7366,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
         <v>4</v>
       </c>
@@ -7395,7 +7401,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
         <v>4</v>
       </c>
@@ -7430,7 +7436,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
         <v>4</v>
       </c>
@@ -7465,7 +7471,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
         <v>4</v>
       </c>
@@ -7500,7 +7506,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
         <v>4</v>
       </c>
@@ -7535,7 +7541,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
         <v>4</v>
       </c>
@@ -7570,7 +7576,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
         <v>4</v>
       </c>
@@ -7605,7 +7611,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
         <v>4</v>
       </c>
@@ -7640,7 +7646,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
         <v>4</v>
       </c>
@@ -7675,7 +7681,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
         <v>4</v>
       </c>
@@ -7710,7 +7716,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
         <v>4</v>
       </c>
@@ -7745,7 +7751,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
         <v>4</v>
       </c>
@@ -7780,7 +7786,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
         <v>4</v>
       </c>
@@ -7815,7 +7821,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
         <v>4</v>
       </c>
@@ -7850,7 +7856,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
         <v>4</v>
       </c>
@@ -7885,7 +7891,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" s="7" t="s">
         <v>4</v>
       </c>
@@ -7920,7 +7926,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="s">
         <v>4</v>
       </c>
@@ -7955,7 +7961,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" s="7" t="s">
         <v>4</v>
       </c>
@@ -7990,7 +7996,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" s="7" t="s">
         <v>4</v>
       </c>
@@ -8025,7 +8031,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" s="7" t="s">
         <v>4</v>
       </c>
@@ -8060,7 +8066,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
         <v>4</v>
       </c>
@@ -8095,7 +8101,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" s="7" t="s">
         <v>4</v>
       </c>
@@ -8130,7 +8136,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
         <v>4</v>
       </c>
@@ -8165,7 +8171,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
         <v>4</v>
       </c>
@@ -8200,7 +8206,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
         <v>4</v>
       </c>
@@ -8235,7 +8241,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
         <v>4</v>
       </c>
@@ -8270,7 +8276,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="s">
         <v>4</v>
       </c>
@@ -8305,7 +8311,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" s="7" t="s">
         <v>4</v>
       </c>
@@ -8340,7 +8346,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" s="7" t="s">
         <v>4</v>
       </c>
@@ -8375,7 +8381,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" s="7" t="s">
         <v>4</v>
       </c>
@@ -8410,7 +8416,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" s="7" t="s">
         <v>4</v>
       </c>
@@ -8445,7 +8451,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" s="7" t="s">
         <v>4</v>
       </c>
@@ -8480,7 +8486,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
         <v>4</v>
       </c>
@@ -8515,7 +8521,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
         <v>4</v>
       </c>
@@ -8550,7 +8556,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="s">
         <v>4</v>
       </c>
@@ -8585,7 +8591,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
         <v>4</v>
       </c>
@@ -8620,7 +8626,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="s">
         <v>4</v>
       </c>
@@ -8655,7 +8661,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" s="7" t="s">
         <v>4</v>
       </c>
@@ -8690,7 +8696,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" s="7" t="s">
         <v>4</v>
       </c>
@@ -8725,7 +8731,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" s="7" t="s">
         <v>4</v>
       </c>
@@ -8760,7 +8766,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" s="7" t="s">
         <v>4</v>
       </c>
@@ -8795,7 +8801,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" s="7" t="s">
         <v>4</v>
       </c>
@@ -8830,7 +8836,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="s">
         <v>4</v>
       </c>
@@ -8865,7 +8871,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
         <v>4</v>
       </c>
@@ -8900,7 +8906,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="s">
         <v>4</v>
       </c>
@@ -8935,7 +8941,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" s="7" t="s">
         <v>4</v>
       </c>
@@ -8970,7 +8976,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="s">
         <v>4</v>
       </c>
@@ -9005,7 +9011,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" s="7" t="s">
         <v>4</v>
       </c>
@@ -9040,7 +9046,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" s="7" t="s">
         <v>4</v>
       </c>
@@ -9075,7 +9081,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" s="7" t="s">
         <v>4</v>
       </c>
@@ -9110,7 +9116,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" s="7" t="s">
         <v>4</v>
       </c>
@@ -9145,7 +9151,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" s="7" t="s">
         <v>4</v>
       </c>
@@ -9180,7 +9186,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
         <v>4</v>
       </c>
@@ -9215,7 +9221,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
         <v>4</v>
       </c>
@@ -9250,7 +9256,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" s="7" t="s">
         <v>4</v>
       </c>
@@ -9285,7 +9291,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
         <v>41</v>
       </c>
@@ -9320,7 +9326,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
         <v>25</v>
       </c>
@@ -9355,7 +9361,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
         <v>25</v>
       </c>
@@ -9390,7 +9396,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
         <v>25</v>
       </c>
@@ -9425,7 +9431,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
         <v>25</v>
       </c>
@@ -9460,7 +9466,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="s">
         <v>25</v>
       </c>
@@ -9495,7 +9501,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
         <v>25</v>
       </c>
@@ -9530,7 +9536,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="s">
         <v>25</v>
       </c>
@@ -9565,7 +9571,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" s="7" t="s">
         <v>25</v>
       </c>
@@ -9600,7 +9606,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" s="7" t="s">
         <v>25</v>
       </c>
@@ -9635,7 +9641,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196" s="7" t="s">
         <v>25</v>
       </c>
@@ -9670,7 +9676,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" s="7" t="s">
         <v>25</v>
       </c>
@@ -9705,7 +9711,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" s="7" t="s">
         <v>130</v>
       </c>
@@ -9740,7 +9746,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" s="7" t="s">
         <v>130</v>
       </c>
@@ -9775,7 +9781,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200" s="7" t="s">
         <v>83</v>
       </c>
@@ -9810,7 +9816,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201" s="7" t="s">
         <v>83</v>
       </c>
@@ -9845,7 +9851,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202" s="7" t="s">
         <v>83</v>
       </c>
@@ -9880,7 +9886,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" s="7" t="s">
         <v>83</v>
       </c>
@@ -9915,7 +9921,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204" s="7" t="s">
         <v>83</v>
       </c>
@@ -9950,7 +9956,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" s="7" t="s">
         <v>111</v>
       </c>
@@ -9985,7 +9991,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206" s="7" t="s">
         <v>111</v>
       </c>
@@ -10020,7 +10026,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207" s="7" t="s">
         <v>59</v>
       </c>
@@ -10055,7 +10061,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" s="7" t="s">
         <v>21</v>
       </c>
@@ -10090,7 +10096,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209" s="7" t="s">
         <v>21</v>
       </c>
@@ -10125,7 +10131,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" s="7" t="s">
         <v>21</v>
       </c>
@@ -10160,7 +10166,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" s="7" t="s">
         <v>21</v>
       </c>
@@ -10195,7 +10201,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212" s="7" t="s">
         <v>21</v>
       </c>
@@ -10230,7 +10236,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" s="7" t="s">
         <v>21</v>
       </c>
@@ -10265,7 +10271,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214" s="7" t="s">
         <v>21</v>
       </c>
@@ -10300,7 +10306,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" s="7" t="s">
         <v>21</v>
       </c>
@@ -10335,7 +10341,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" s="7" t="s">
         <v>21</v>
       </c>
@@ -10370,7 +10376,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217" s="7" t="s">
         <v>15</v>
       </c>
@@ -10405,7 +10411,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218" s="7" t="s">
         <v>15</v>
       </c>
@@ -10440,7 +10446,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219" s="7" t="s">
         <v>15</v>
       </c>
@@ -10475,7 +10481,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" s="7" t="s">
         <v>15</v>
       </c>
@@ -10510,7 +10516,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" s="7" t="s">
         <v>15</v>
       </c>
@@ -10545,7 +10551,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" s="7" t="s">
         <v>15</v>
       </c>
@@ -10580,7 +10586,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" s="7" t="s">
         <v>15</v>
       </c>
@@ -10615,7 +10621,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" s="7" t="s">
         <v>15</v>
       </c>
@@ -10650,7 +10656,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" s="7" t="s">
         <v>15</v>
       </c>
@@ -10685,7 +10691,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" s="7" t="s">
         <v>15</v>
       </c>
@@ -10720,7 +10726,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227" s="7" t="s">
         <v>15</v>
       </c>
@@ -10755,7 +10761,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228" s="7" t="s">
         <v>15</v>
       </c>
@@ -10790,7 +10796,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" s="7" t="s">
         <v>15</v>
       </c>
@@ -10825,7 +10831,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" s="7" t="s">
         <v>15</v>
       </c>
@@ -10860,7 +10866,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>15</v>
       </c>
@@ -10895,7 +10901,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="232" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="7" t="s">
         <v>29</v>
       </c>
@@ -10930,7 +10936,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233" s="7" t="s">
         <v>10</v>
       </c>
@@ -10965,7 +10971,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234" s="7" t="s">
         <v>10</v>
       </c>
@@ -11000,7 +11006,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235" s="7" t="s">
         <v>10</v>
       </c>
@@ -11035,7 +11041,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236" s="7" t="s">
         <v>10</v>
       </c>
@@ -11070,7 +11076,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237" s="7" t="s">
         <v>10</v>
       </c>
@@ -11105,7 +11111,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238" s="7" t="s">
         <v>10</v>
       </c>
@@ -11140,7 +11146,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239" s="7" t="s">
         <v>10</v>
       </c>
@@ -11175,7 +11181,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240" s="7" t="s">
         <v>10</v>
       </c>
@@ -11210,7 +11216,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241" s="7" t="s">
         <v>10</v>
       </c>
@@ -11245,7 +11251,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242" s="7" t="s">
         <v>10</v>
       </c>
@@ -11280,7 +11286,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243" s="7" t="s">
         <v>10</v>
       </c>
@@ -11315,7 +11321,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244" s="7" t="s">
         <v>10</v>
       </c>
@@ -11350,7 +11356,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245" s="7" t="s">
         <v>10</v>
       </c>
@@ -11385,7 +11391,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246" s="7" t="s">
         <v>10</v>
       </c>
@@ -11420,7 +11426,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247" s="7" t="s">
         <v>10</v>
       </c>
@@ -11455,7 +11461,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248" s="7" t="s">
         <v>10</v>
       </c>
@@ -11490,7 +11496,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249" s="7" t="s">
         <v>10</v>
       </c>
@@ -11525,7 +11531,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250" s="7" t="s">
         <v>10</v>
       </c>
@@ -11560,7 +11566,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251" s="7" t="s">
         <v>10</v>
       </c>
@@ -11595,7 +11601,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252" s="7" t="s">
         <v>10</v>
       </c>
@@ -11630,7 +11636,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253" s="7" t="s">
         <v>10</v>
       </c>
@@ -11665,7 +11671,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A254" s="7" t="s">
         <v>10</v>
       </c>
@@ -11700,7 +11706,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255" s="7" t="s">
         <v>10</v>
       </c>
@@ -11735,7 +11741,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A256" s="7" t="s">
         <v>10</v>
       </c>
@@ -11770,7 +11776,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257" s="7" t="s">
         <v>10</v>
       </c>

</xml_diff>